<commit_message>
added colors to python and js
</commit_message>
<xml_diff>
--- a/data/manual/hrafnkel_saga_network_with_flags_colors.xlsx
+++ b/data/manual/hrafnkel_saga_network_with_flags_colors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Moritz/Documents/TU/GD_Graph Drawing Algorithms/hrafnkel/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Moritz/Documents/TU/GD_Graph Drawing Algorithms/hrafnkel/data/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19720328-D3AA-2048-82EE-9DA7E062398F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF535F6B-7D0A-7B43-947C-65C31358E2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,18 +57,6 @@
     <t>page</t>
   </si>
   <si>
-    <t>weight in</t>
-  </si>
-  <si>
-    <t>weight out</t>
-  </si>
-  <si>
-    <t>only once</t>
-  </si>
-  <si>
-    <t>never used</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
@@ -553,6 +541,18 @@
   </si>
   <si>
     <t>notes</t>
+  </si>
+  <si>
+    <t>is_never</t>
+  </si>
+  <si>
+    <t>weight_out</t>
+  </si>
+  <si>
+    <t>weight_in</t>
+  </si>
+  <si>
+    <t>is_one_time</t>
   </si>
 </sst>
 </file>
@@ -943,7 +943,7 @@
   <dimension ref="A1:L44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,25 +973,25 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>169</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>168</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>170</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>167</v>
       </c>
       <c r="J1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="K1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1020,10 +1020,10 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1034,7 +1034,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1052,10 +1052,10 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -1066,7 +1066,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1084,10 +1084,10 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1098,7 +1098,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1116,10 +1116,10 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1148,10 +1148,10 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L6">
         <v>0</v>
@@ -1162,7 +1162,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1183,10 +1183,10 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L7">
         <v>0</v>
@@ -1197,7 +1197,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1215,10 +1215,10 @@
         <v>6</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1229,7 +1229,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1247,10 +1247,10 @@
         <v>1</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1261,7 +1261,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1279,10 +1279,10 @@
         <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1293,7 +1293,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1311,10 +1311,10 @@
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L11" s="2">
         <v>6</v>
@@ -1325,7 +1325,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1346,10 +1346,10 @@
         <v>1</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L12">
         <v>6</v>
@@ -1360,7 +1360,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1378,10 +1378,10 @@
         <v>2</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1392,7 +1392,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1410,10 +1410,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1424,7 +1424,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1442,10 +1442,10 @@
         <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -1456,7 +1456,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1474,10 +1474,10 @@
         <v>2</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L16">
         <v>7</v>
@@ -1488,7 +1488,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1506,10 +1506,10 @@
         <v>3</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L17">
         <v>2</v>
@@ -1520,7 +1520,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1532,10 +1532,10 @@
         <v>2</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="L18">
         <v>2</v>
@@ -1546,7 +1546,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1564,10 +1564,10 @@
         <v>16</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="L19">
         <v>2</v>
@@ -1578,7 +1578,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1590,10 +1590,10 @@
         <v>5</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="L20">
         <v>2</v>
@@ -1604,7 +1604,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1625,10 +1625,10 @@
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="L21">
         <v>2</v>
@@ -1639,7 +1639,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -1651,10 +1651,10 @@
         <v>5</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L22">
         <v>6</v>
@@ -1665,7 +1665,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1677,10 +1677,10 @@
         <v>3</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="L23">
         <v>7</v>
@@ -1691,7 +1691,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1709,10 +1709,10 @@
         <v>4</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L24">
         <v>2</v>
@@ -1723,7 +1723,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1741,10 +1741,10 @@
         <v>6</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="L25">
         <v>2</v>
@@ -1755,7 +1755,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -1767,10 +1767,10 @@
         <v>2</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L26">
         <v>6</v>
@@ -1781,7 +1781,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1793,10 +1793,10 @@
         <v>2</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L27">
         <v>6</v>
@@ -1807,7 +1807,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1822,10 +1822,10 @@
         <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L28">
         <v>6</v>
@@ -1836,7 +1836,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1851,10 +1851,10 @@
         <v>1</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L29">
         <v>6</v>
@@ -1865,7 +1865,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1883,10 +1883,10 @@
         <v>4</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L30">
         <v>3</v>
@@ -1897,7 +1897,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1909,10 +1909,10 @@
         <v>3</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="L31">
         <v>3</v>
@@ -1923,7 +1923,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1941,10 +1941,10 @@
         <v>7</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L32">
         <v>3</v>
@@ -1955,7 +1955,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -1973,10 +1973,10 @@
         <v>0</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="L33">
         <v>3</v>
@@ -1987,7 +1987,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2005,10 +2005,10 @@
         <v>1</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L34">
         <v>3</v>
@@ -2019,7 +2019,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2040,10 +2040,10 @@
         <v>1</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="L35">
         <v>3</v>
@@ -2054,7 +2054,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2072,10 +2072,10 @@
         <v>1</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="L36">
         <v>2</v>
@@ -2086,7 +2086,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2104,10 +2104,10 @@
         <v>0</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L37">
         <v>6</v>
@@ -2118,7 +2118,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2139,10 +2139,10 @@
         <v>1</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L38">
         <v>4</v>
@@ -2153,7 +2153,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2174,10 +2174,10 @@
         <v>1</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L39">
         <v>4</v>
@@ -2188,7 +2188,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2203,10 +2203,10 @@
         <v>1</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="L40">
         <v>4</v>
@@ -2217,7 +2217,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2232,10 +2232,10 @@
         <v>1</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="L41">
         <v>5</v>
@@ -2246,7 +2246,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2267,10 +2267,10 @@
         <v>1</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L42">
         <v>5</v>
@@ -2281,7 +2281,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2302,10 +2302,10 @@
         <v>1</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="L43">
         <v>5</v>
@@ -2316,7 +2316,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2331,10 +2331,10 @@
         <v>1</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="L44">
         <v>6</v>
@@ -2361,13 +2361,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2375,7 +2375,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2383,7 +2383,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2391,7 +2391,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2399,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2407,7 +2407,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2415,7 +2415,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2423,10 +2423,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2434,10 +2434,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
@@ -2470,13 +2470,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -4736,10 +4736,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -4747,7 +4747,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4755,7 +4755,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -4763,7 +4763,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -4771,7 +4771,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -4779,7 +4779,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -4787,7 +4787,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -4795,7 +4795,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -4803,7 +4803,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -4811,7 +4811,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -4819,7 +4819,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -4827,7 +4827,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -4835,7 +4835,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -4843,7 +4843,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -4851,7 +4851,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -4859,7 +4859,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -4867,7 +4867,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -4875,7 +4875,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -4883,7 +4883,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -4891,7 +4891,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -4899,7 +4899,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -4907,7 +4907,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -4915,7 +4915,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -4923,7 +4923,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -4931,7 +4931,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -4939,7 +4939,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -4947,7 +4947,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -4955,7 +4955,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -4963,7 +4963,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -4971,7 +4971,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -4998,7 +4998,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -5006,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5014,7 +5014,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -5022,7 +5022,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fonts, pdfs final versions
</commit_message>
<xml_diff>
--- a/data/manual/hrafnkel_saga_network_with_flags_colors.xlsx
+++ b/data/manual/hrafnkel_saga_network_with_flags_colors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Moritz/Documents/TU/GD_Graph Drawing Algorithms/hrafnkel/data/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F3A1A4-1227-4943-85F8-250F4569944B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757E4553-D4FA-3441-A643-B4C4345E0128}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21780" windowHeight="19880" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1086,7 +1086,7 @@
   <dimension ref="A1:O46"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4822,8 +4822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>